<commit_message>
logs cleaning and sorting
</commit_message>
<xml_diff>
--- a/server/helpers/registration.xlsx
+++ b/server/helpers/registration.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/migleberesineviciute/Documents/GitHub/omnium/server/helpers/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{989BB17E-16BC-0C43-8E6A-BE9B72AEA262}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{638C5D38-B2F6-E549-951C-7AAFA44B943A}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1860" yWindow="2080" windowWidth="14400" windowHeight="12860" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1860" yWindow="2080" windowWidth="26940" windowHeight="13080" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="registration" sheetId="1" r:id="rId1"/>
@@ -353,10 +353,10 @@
     <t>Julia</t>
   </si>
   <si>
-    <t>TEST</t>
-  </si>
-  <si>
-    <t>Tdest</t>
+    <t>TESTtte</t>
+  </si>
+  <si>
+    <t>Tdester</t>
   </si>
 </sst>
 </file>
@@ -718,8 +718,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:J23"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="D9" sqref="D9"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H15" sqref="H15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -765,7 +765,7 @@
         <v>111</v>
       </c>
       <c r="D2">
-        <v>123455432</v>
+        <v>120005432</v>
       </c>
       <c r="E2" t="s">
         <v>8</v>

</xml_diff>

<commit_message>
validation for file upload
</commit_message>
<xml_diff>
--- a/server/helpers/registration.xlsx
+++ b/server/helpers/registration.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/migleberesineviciute/Documents/GitHub/omnium/server/helpers/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{638C5D38-B2F6-E549-951C-7AAFA44B943A}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{54BD87BE-DA86-FC4E-9A41-B6D98ACC2B1E}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1860" yWindow="2080" windowWidth="26940" windowHeight="13080" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="258" uniqueCount="112">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="270" uniqueCount="114">
   <si>
     <t>First name</t>
   </si>
@@ -357,6 +357,12 @@
   </si>
   <si>
     <t>Tdester</t>
+  </si>
+  <si>
+    <t xml:space="preserve">POOd .djsjs </t>
+  </si>
+  <si>
+    <t>selrect * from "Top"</t>
   </si>
 </sst>
 </file>
@@ -719,7 +725,7 @@
   <dimension ref="A1:J23"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H15" sqref="H15"/>
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -765,7 +771,7 @@
         <v>111</v>
       </c>
       <c r="D2">
-        <v>120005432</v>
+        <v>91200054323</v>
       </c>
       <c r="E2" t="s">
         <v>8</v>
@@ -780,6 +786,64 @@
         <v>56</v>
       </c>
       <c r="I2" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A3">
+        <v>2</v>
+      </c>
+      <c r="B3" t="s">
+        <v>112</v>
+      </c>
+      <c r="C3" t="s">
+        <v>113</v>
+      </c>
+      <c r="D3">
+        <v>234</v>
+      </c>
+      <c r="E3" t="s">
+        <v>8</v>
+      </c>
+      <c r="F3" t="s">
+        <v>8</v>
+      </c>
+      <c r="G3" s="3">
+        <v>35697</v>
+      </c>
+      <c r="H3" t="s">
+        <v>56</v>
+      </c>
+      <c r="I3" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A4" s="1">
+        <v>10</v>
+      </c>
+      <c r="B4" t="s">
+        <v>47</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="D4">
+        <v>10009084739</v>
+      </c>
+      <c r="E4" t="s">
+        <v>49</v>
+      </c>
+      <c r="F4" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="G4" s="2">
+        <v>35195</v>
+      </c>
+      <c r="H4" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="I4" s="1" t="s">
         <v>44</v>
       </c>
     </row>
@@ -812,7 +876,7 @@
   <dimension ref="A1:J49"/>
   <sheetViews>
     <sheetView topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="D28" sqref="D28"/>
+      <selection activeCell="A11" sqref="A11:I11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0.15"/>

</xml_diff>